<commit_message>
Events Filter is pending
Everything else done for iteration 1
</commit_message>
<xml_diff>
--- a/Documents/Work Breakdown Iteration 1.xlsx
+++ b/Documents/Work Breakdown Iteration 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/eldvisor/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D602BC-9EC1-4C4D-80C5-E8E04BD7A05F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C68DEDE-109B-3246-8FF1-49E172EADFE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1994,7 +1994,67 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2228,8 +2288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2237,7 +2297,7 @@
     <col min="1" max="1" width="108.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="84.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="19" width="7.6640625" customWidth="1"/>
   </cols>
@@ -2277,7 +2337,7 @@
       </c>
       <c r="F2">
         <f>COUNTIF(C:C,"Done")</f>
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.2">
@@ -2295,7 +2355,7 @@
       </c>
       <c r="F3">
         <f>COUNTIF(C:C,"Doing")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
@@ -2314,7 +2374,7 @@
       </c>
       <c r="F4">
         <f>COUNTIF(C:C,"To-Do")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="150" x14ac:dyDescent="0.2">
@@ -2518,7 +2578,7 @@
         <v>35</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.2">
@@ -2529,7 +2589,7 @@
         <v>36</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2540,7 +2600,7 @@
         <v>37</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.2">
@@ -2551,7 +2611,7 @@
         <v>38</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.2">
@@ -2562,7 +2622,7 @@
         <v>39</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3540,10 +3600,10 @@
   </sheetData>
   <autoFilter ref="A1:B28" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="C29:C1048576 C2:C26">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>